<commit_message>
Updated formal attendance record
</commit_message>
<xml_diff>
--- a/doc/Formal-Attendance.xlsx
+++ b/doc/Formal-Attendance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="23">
   <si>
     <t>Formal Meetings</t>
   </si>
@@ -45,12 +45,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
     <t>Column3</t>
   </si>
   <si>
@@ -82,6 +76,15 @@
   </si>
   <si>
     <t>4/12/2009</t>
+  </si>
+  <si>
+    <t>17/2/20102</t>
+  </si>
+  <si>
+    <t>2/2/2010</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -124,19 +127,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <condense val="0"/>
@@ -177,8 +168,8 @@
     <tableColumn id="5" name="11/11/2009"/>
     <tableColumn id="6" name="30/11/2009"/>
     <tableColumn id="7" name="4/12/2009"/>
-    <tableColumn id="8" name="Column1"/>
-    <tableColumn id="9" name="Column2"/>
+    <tableColumn id="8" name="2/2/2010"/>
+    <tableColumn id="9" name="17/2/20102"/>
     <tableColumn id="10" name="Column3"/>
     <tableColumn id="11" name="Column4"/>
     <tableColumn id="12" name="Column5"/>
@@ -477,7 +468,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -496,43 +487,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -557,6 +548,12 @@
       <c r="G3" t="s">
         <v>7</v>
       </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
@@ -580,6 +577,12 @@
       <c r="G4" t="s">
         <v>7</v>
       </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
@@ -603,6 +606,12 @@
       <c r="G5" t="s">
         <v>7</v>
       </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
@@ -626,6 +635,12 @@
       <c r="G6" t="s">
         <v>7</v>
       </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
@@ -649,6 +664,12 @@
       <c r="G7" t="s">
         <v>7</v>
       </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
@@ -672,13 +693,19 @@
       <c r="G8" t="s">
         <v>7</v>
       </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:N8">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="*-*">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="*-*">
       <formula>NOT(ISERROR(SEARCH("*-*",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",B3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated the Formal attendance list.
</commit_message>
<xml_diff>
--- a/doc/Formal-Attendance.xlsx
+++ b/doc/Formal-Attendance.xlsx
@@ -468,7 +468,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -561,7 +561,7 @@
         <v>7</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="M3" t="s">
         <v>18</v>
@@ -602,7 +602,7 @@
         <v>8</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="M4" t="s">
         <v>18</v>
@@ -643,7 +643,7 @@
         <v>7</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="M5" t="s">
         <v>18</v>
@@ -684,7 +684,7 @@
         <v>8</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="M6" t="s">
         <v>18</v>
@@ -725,7 +725,7 @@
         <v>7</v>
       </c>
       <c r="L7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="M7" t="s">
         <v>18</v>
@@ -766,7 +766,7 @@
         <v>7</v>
       </c>
       <c r="L8" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="M8" t="s">
         <v>18</v>

</xml_diff>